<commit_message>
Credentials for LTRSPG-2212 dCloud Lab
</commit_message>
<xml_diff>
--- a/LTRSPG-2212 dCloud Credentials.xlsx
+++ b/LTRSPG-2212 dCloud Credentials.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robermur/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robermur/Projects/SRv6_dCloud_Lab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA37A816-8172-4606-92AD-E3A6B531DA79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C834D6-F83F-E449-999D-837F9247FD25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{D888498A-EEF0-1E4D-8E3D-FA3DF4C03B65}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="46">
   <si>
     <t>Student</t>
   </si>
@@ -174,34 +174,13 @@
   </si>
   <si>
     <t>917a8a</t>
-  </si>
-  <si>
-    <t>RESERVED</t>
-  </si>
-  <si>
-    <t>v1766user1</t>
-  </si>
-  <si>
-    <t>6c1c83</t>
-  </si>
-  <si>
-    <t>v2822user1</t>
-  </si>
-  <si>
-    <t>d65bd2</t>
-  </si>
-  <si>
-    <t>v1785user1</t>
-  </si>
-  <si>
-    <t>67c2d9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -337,8 +316,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B21B7F16-29FE-4C40-8941-CE83ADC98115}" name="Table1" displayName="Table1" ref="B1:F24" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="B1:F24" xr:uid="{B21B7F16-29FE-4C40-8941-CE83ADC98115}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B21B7F16-29FE-4C40-8941-CE83ADC98115}" name="Table1" displayName="Table1" ref="B1:F21" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="B1:F21" xr:uid="{B21B7F16-29FE-4C40-8941-CE83ADC98115}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -655,25 +634,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF912A64-1F50-B343-B756-59A4D1E604CC}">
-  <dimension ref="B1:F24"/>
+  <dimension ref="B1:F21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34.875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.75" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14.25" style="2" customWidth="1"/>
-    <col min="6" max="6" width="23.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" s="4" customFormat="1" ht="18">
+    <row r="1" spans="2:6" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
@@ -690,7 +669,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" s="2">
         <v>1</v>
       </c>
@@ -707,7 +686,7 @@
         <v>603484</v>
       </c>
     </row>
-    <row r="3" spans="2:6">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="2">
         <v>2</v>
       </c>
@@ -725,7 +704,7 @@
         <v>603483</v>
       </c>
     </row>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" s="2">
         <v>3</v>
       </c>
@@ -739,11 +718,11 @@
         <v>11</v>
       </c>
       <c r="F4" s="3">
-        <f t="shared" ref="F4:F24" si="0">F3-1</f>
+        <f t="shared" ref="F4:F21" si="0">F3-1</f>
         <v>603482</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <v>4</v>
       </c>
@@ -761,7 +740,7 @@
         <v>603481</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="2">
         <v>5</v>
       </c>
@@ -779,7 +758,7 @@
         <v>603480</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
         <v>6</v>
       </c>
@@ -797,7 +776,7 @@
         <v>603479</v>
       </c>
     </row>
-    <row r="8" spans="2:6">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
         <v>7</v>
       </c>
@@ -815,7 +794,7 @@
         <v>603478</v>
       </c>
     </row>
-    <row r="9" spans="2:6">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
         <v>8</v>
       </c>
@@ -833,7 +812,7 @@
         <v>603477</v>
       </c>
     </row>
-    <row r="10" spans="2:6">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
         <v>9</v>
       </c>
@@ -851,7 +830,7 @@
         <v>603476</v>
       </c>
     </row>
-    <row r="11" spans="2:6">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" s="2">
         <v>10</v>
       </c>
@@ -869,7 +848,7 @@
         <v>603475</v>
       </c>
     </row>
-    <row r="12" spans="2:6">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" s="2">
         <v>11</v>
       </c>
@@ -887,7 +866,7 @@
         <v>603474</v>
       </c>
     </row>
-    <row r="13" spans="2:6">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
         <v>12</v>
       </c>
@@ -905,7 +884,7 @@
         <v>603473</v>
       </c>
     </row>
-    <row r="14" spans="2:6">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B14" s="2">
         <v>13</v>
       </c>
@@ -923,7 +902,7 @@
         <v>603472</v>
       </c>
     </row>
-    <row r="15" spans="2:6">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
         <v>14</v>
       </c>
@@ -941,7 +920,7 @@
         <v>603471</v>
       </c>
     </row>
-    <row r="16" spans="2:6">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B16" s="2">
         <v>15</v>
       </c>
@@ -959,7 +938,7 @@
         <v>603470</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" s="2">
         <v>16</v>
       </c>
@@ -977,7 +956,7 @@
         <v>603469</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" s="2">
         <v>17</v>
       </c>
@@ -995,7 +974,7 @@
         <v>603468</v>
       </c>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" s="2">
         <v>18</v>
       </c>
@@ -1013,7 +992,7 @@
         <v>603467</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" s="2">
         <v>19</v>
       </c>
@@ -1031,7 +1010,7 @@
         <v>603466</v>
       </c>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
         <v>20</v>
       </c>
@@ -1047,60 +1026,6 @@
       <c r="F21" s="3">
         <f t="shared" si="0"/>
         <v>603465</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6">
-      <c r="B22" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F22" s="3">
-        <f t="shared" si="0"/>
-        <v>603464</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6">
-      <c r="B23" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23" s="3">
-        <f t="shared" si="0"/>
-        <v>603463</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6">
-      <c r="B24" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F24" s="3">
-        <f t="shared" si="0"/>
-        <v>603462</v>
       </c>
     </row>
   </sheetData>
@@ -1112,6 +1037,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <OriginalAuthor xmlns="ef37b0e3-18cb-42f9-b8cf-c7da6afc8994" xsi:nil="true"/>
@@ -1122,15 +1056,6 @@
     <TaxCatchAll xmlns="18ee132d-42b1-40b5-95fb-8ae7263f7070" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1383,13 +1308,39 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{068EA16F-BBC5-4DF0-9CC7-BACD9871504C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9FA7C18-5857-45DA-93DB-45E45F62706C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A9FA7C18-5857-45DA-93DB-45E45F62706C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{068EA16F-BBC5-4DF0-9CC7-BACD9871504C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ef37b0e3-18cb-42f9-b8cf-c7da6afc8994"/>
+    <ds:schemaRef ds:uri="18ee132d-42b1-40b5-95fb-8ae7263f7070"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3582D3EB-0477-46E5-9473-B7AE5C86D612}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3582D3EB-0477-46E5-9473-B7AE5C86D612}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ef37b0e3-18cb-42f9-b8cf-c7da6afc8994"/>
+    <ds:schemaRef ds:uri="18ee132d-42b1-40b5-95fb-8ae7263f7070"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>